<commit_message>
Modifications to data version 2. Ony renaming for version 1. Summing it up for version 2: 50 trucks considered, 10 trucks per depot (5 depots).
</commit_message>
<xml_diff>
--- a/data/initial_data_info.xlsx
+++ b/data/initial_data_info.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clara.gregori\projects\VisualStudioCode\routing-model-2025\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C77ED9D1-50FB-4B26-A2A1-CF3E1857832D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3717B6D-A8B6-4BA2-9110-A1F20361DE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="5" xr2:uid="{9F6578B3-E217-4A8C-A4A8-11896FE55B29}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9F6578B3-E217-4A8C-A4A8-11896FE55B29}"/>
   </bookViews>
   <sheets>
     <sheet name="trucks" sheetId="1" r:id="rId1"/>
     <sheet name="pallets" sheetId="2" r:id="rId2"/>
-    <sheet name="depot" sheetId="4" r:id="rId3"/>
-    <sheet name="customer" sheetId="5" r:id="rId4"/>
+    <sheet name="depots" sheetId="4" r:id="rId3"/>
+    <sheet name="customers" sheetId="5" r:id="rId4"/>
     <sheet name="products" sheetId="3" r:id="rId5"/>
     <sheet name="OLDdistances_depot_costumers" sheetId="7" r:id="rId6"/>
     <sheet name="commands_v0" sheetId="6" r:id="rId7"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8113" uniqueCount="4055">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8231" uniqueCount="4058">
   <si>
     <t>F1</t>
   </si>
@@ -12348,6 +12348,15 @@
   </si>
   <si>
     <t>EuropeoPetf2</t>
+  </si>
+  <si>
+    <t>id_type</t>
+  </si>
+  <si>
+    <t>F4</t>
+  </si>
+  <si>
+    <t>F5</t>
   </si>
 </sst>
 </file>
@@ -12807,104 +12816,1423 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B4B57A9-B49C-41B3-B600-93F9DD029928}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="11.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.33203125" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4022</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4055</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>4034</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>4035</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>4036</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>4037</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="G1" s="1" t="s">
+        <v>4024</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>4044</v>
       </c>
-      <c r="B2">
+      <c r="C2">
         <v>15000</v>
       </c>
-      <c r="C2">
+      <c r="D2">
         <v>2.5</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>9.5</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="G2" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
         <v>4045</v>
       </c>
-      <c r="B3">
+      <c r="C3">
         <v>24000</v>
       </c>
-      <c r="C3">
+      <c r="D3">
         <v>2.5</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>11</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
+      <c r="G3" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
         <v>4046</v>
       </c>
-      <c r="B4">
+      <c r="C4">
         <v>27000</v>
       </c>
-      <c r="C4">
+      <c r="D4">
         <v>2.5</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>13.6</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>2.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+      <c r="G4" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
         <v>4047</v>
       </c>
-      <c r="B5">
+      <c r="C5">
         <v>10000</v>
       </c>
-      <c r="C5">
+      <c r="D5">
         <v>2.5</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>7.5</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>2.5</v>
       </c>
+      <c r="G5" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C6">
+        <v>10000</v>
+      </c>
+      <c r="D6">
+        <v>2.5</v>
+      </c>
+      <c r="E6">
+        <v>7.5</v>
+      </c>
+      <c r="F6">
+        <v>2.5</v>
+      </c>
+      <c r="G6" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>4044</v>
+      </c>
+      <c r="C7">
+        <v>15000</v>
+      </c>
+      <c r="D7">
+        <v>2.5</v>
+      </c>
+      <c r="E7">
+        <v>9.5</v>
+      </c>
+      <c r="F7">
+        <v>2.5</v>
+      </c>
+      <c r="G7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" t="s">
+        <v>4045</v>
+      </c>
+      <c r="C8">
+        <v>24000</v>
+      </c>
+      <c r="D8">
+        <v>2.5</v>
+      </c>
+      <c r="E8">
+        <v>11</v>
+      </c>
+      <c r="F8">
+        <v>2.5</v>
+      </c>
+      <c r="G8" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" t="s">
+        <v>4046</v>
+      </c>
+      <c r="C9">
+        <v>27000</v>
+      </c>
+      <c r="D9">
+        <v>2.5</v>
+      </c>
+      <c r="E9">
+        <v>13.6</v>
+      </c>
+      <c r="F9">
+        <v>2.5</v>
+      </c>
+      <c r="G9" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C10">
+        <v>10000</v>
+      </c>
+      <c r="D10">
+        <v>2.5</v>
+      </c>
+      <c r="E10">
+        <v>7.5</v>
+      </c>
+      <c r="F10">
+        <v>2.5</v>
+      </c>
+      <c r="G10" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C11">
+        <v>10000</v>
+      </c>
+      <c r="D11">
+        <v>2.5</v>
+      </c>
+      <c r="E11">
+        <v>7.5</v>
+      </c>
+      <c r="F11">
+        <v>2.5</v>
+      </c>
+      <c r="G11" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>4044</v>
+      </c>
+      <c r="C12">
+        <v>15000</v>
+      </c>
+      <c r="D12">
+        <v>2.5</v>
+      </c>
+      <c r="E12">
+        <v>9.5</v>
+      </c>
+      <c r="F12">
+        <v>2.5</v>
+      </c>
+      <c r="G12" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4045</v>
+      </c>
+      <c r="C13">
+        <v>24000</v>
+      </c>
+      <c r="D13">
+        <v>2.5</v>
+      </c>
+      <c r="E13">
+        <v>11</v>
+      </c>
+      <c r="F13">
+        <v>2.5</v>
+      </c>
+      <c r="G13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>4046</v>
+      </c>
+      <c r="C14">
+        <v>27000</v>
+      </c>
+      <c r="D14">
+        <v>2.5</v>
+      </c>
+      <c r="E14">
+        <v>13.6</v>
+      </c>
+      <c r="F14">
+        <v>2.5</v>
+      </c>
+      <c r="G14" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C15">
+        <v>10000</v>
+      </c>
+      <c r="D15">
+        <v>2.5</v>
+      </c>
+      <c r="E15">
+        <v>7.5</v>
+      </c>
+      <c r="F15">
+        <v>2.5</v>
+      </c>
+      <c r="G15" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C16">
+        <v>10000</v>
+      </c>
+      <c r="D16">
+        <v>2.5</v>
+      </c>
+      <c r="E16">
+        <v>7.5</v>
+      </c>
+      <c r="F16">
+        <v>2.5</v>
+      </c>
+      <c r="G16" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>4044</v>
+      </c>
+      <c r="C17">
+        <v>15000</v>
+      </c>
+      <c r="D17">
+        <v>2.5</v>
+      </c>
+      <c r="E17">
+        <v>9.5</v>
+      </c>
+      <c r="F17">
+        <v>2.5</v>
+      </c>
+      <c r="G17" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
+        <v>4045</v>
+      </c>
+      <c r="C18">
+        <v>24000</v>
+      </c>
+      <c r="D18">
+        <v>2.5</v>
+      </c>
+      <c r="E18">
+        <v>11</v>
+      </c>
+      <c r="F18">
+        <v>2.5</v>
+      </c>
+      <c r="G18" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4046</v>
+      </c>
+      <c r="C19">
+        <v>27000</v>
+      </c>
+      <c r="D19">
+        <v>2.5</v>
+      </c>
+      <c r="E19">
+        <v>13.6</v>
+      </c>
+      <c r="F19">
+        <v>2.5</v>
+      </c>
+      <c r="G19" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C20">
+        <v>10000</v>
+      </c>
+      <c r="D20">
+        <v>2.5</v>
+      </c>
+      <c r="E20">
+        <v>7.5</v>
+      </c>
+      <c r="F20">
+        <v>2.5</v>
+      </c>
+      <c r="G20" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C21">
+        <v>10000</v>
+      </c>
+      <c r="D21">
+        <v>2.5</v>
+      </c>
+      <c r="E21">
+        <v>7.5</v>
+      </c>
+      <c r="F21">
+        <v>2.5</v>
+      </c>
+      <c r="G21" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
+        <v>4044</v>
+      </c>
+      <c r="C22">
+        <v>15000</v>
+      </c>
+      <c r="D22">
+        <v>2.5</v>
+      </c>
+      <c r="E22">
+        <v>9.5</v>
+      </c>
+      <c r="F22">
+        <v>2.5</v>
+      </c>
+      <c r="G22" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>4045</v>
+      </c>
+      <c r="C23">
+        <v>24000</v>
+      </c>
+      <c r="D23">
+        <v>2.5</v>
+      </c>
+      <c r="E23">
+        <v>11</v>
+      </c>
+      <c r="F23">
+        <v>2.5</v>
+      </c>
+      <c r="G23" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4046</v>
+      </c>
+      <c r="C24">
+        <v>27000</v>
+      </c>
+      <c r="D24">
+        <v>2.5</v>
+      </c>
+      <c r="E24">
+        <v>13.6</v>
+      </c>
+      <c r="F24">
+        <v>2.5</v>
+      </c>
+      <c r="G24" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C25">
+        <v>10000</v>
+      </c>
+      <c r="D25">
+        <v>2.5</v>
+      </c>
+      <c r="E25">
+        <v>7.5</v>
+      </c>
+      <c r="F25">
+        <v>2.5</v>
+      </c>
+      <c r="G25" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C26">
+        <v>10000</v>
+      </c>
+      <c r="D26">
+        <v>2.5</v>
+      </c>
+      <c r="E26">
+        <v>7.5</v>
+      </c>
+      <c r="F26">
+        <v>2.5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
+        <v>4044</v>
+      </c>
+      <c r="C27">
+        <v>15000</v>
+      </c>
+      <c r="D27">
+        <v>2.5</v>
+      </c>
+      <c r="E27">
+        <v>9.5</v>
+      </c>
+      <c r="F27">
+        <v>2.5</v>
+      </c>
+      <c r="G27" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4045</v>
+      </c>
+      <c r="C28">
+        <v>24000</v>
+      </c>
+      <c r="D28">
+        <v>2.5</v>
+      </c>
+      <c r="E28">
+        <v>11</v>
+      </c>
+      <c r="F28">
+        <v>2.5</v>
+      </c>
+      <c r="G28" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>4046</v>
+      </c>
+      <c r="C29">
+        <v>27000</v>
+      </c>
+      <c r="D29">
+        <v>2.5</v>
+      </c>
+      <c r="E29">
+        <v>13.6</v>
+      </c>
+      <c r="F29">
+        <v>2.5</v>
+      </c>
+      <c r="G29" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C30">
+        <v>10000</v>
+      </c>
+      <c r="D30">
+        <v>2.5</v>
+      </c>
+      <c r="E30">
+        <v>7.5</v>
+      </c>
+      <c r="F30">
+        <v>2.5</v>
+      </c>
+      <c r="G30" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C31">
+        <v>10000</v>
+      </c>
+      <c r="D31">
+        <v>2.5</v>
+      </c>
+      <c r="E31">
+        <v>7.5</v>
+      </c>
+      <c r="F31">
+        <v>2.5</v>
+      </c>
+      <c r="G31" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>4044</v>
+      </c>
+      <c r="C32">
+        <v>15000</v>
+      </c>
+      <c r="D32">
+        <v>2.5</v>
+      </c>
+      <c r="E32">
+        <v>9.5</v>
+      </c>
+      <c r="F32">
+        <v>2.5</v>
+      </c>
+      <c r="G32" t="s">
+        <v>4056</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
+        <v>4045</v>
+      </c>
+      <c r="C33">
+        <v>24000</v>
+      </c>
+      <c r="D33">
+        <v>2.5</v>
+      </c>
+      <c r="E33">
+        <v>11</v>
+      </c>
+      <c r="F33">
+        <v>2.5</v>
+      </c>
+      <c r="G33" t="s">
+        <v>4056</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
+        <v>4046</v>
+      </c>
+      <c r="C34">
+        <v>27000</v>
+      </c>
+      <c r="D34">
+        <v>2.5</v>
+      </c>
+      <c r="E34">
+        <v>13.6</v>
+      </c>
+      <c r="F34">
+        <v>2.5</v>
+      </c>
+      <c r="G34" t="s">
+        <v>4056</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C35">
+        <v>10000</v>
+      </c>
+      <c r="D35">
+        <v>2.5</v>
+      </c>
+      <c r="E35">
+        <v>7.5</v>
+      </c>
+      <c r="F35">
+        <v>2.5</v>
+      </c>
+      <c r="G35" t="s">
+        <v>4056</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C36">
+        <v>10000</v>
+      </c>
+      <c r="D36">
+        <v>2.5</v>
+      </c>
+      <c r="E36">
+        <v>7.5</v>
+      </c>
+      <c r="F36">
+        <v>2.5</v>
+      </c>
+      <c r="G36" t="s">
+        <v>4056</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
+        <v>4044</v>
+      </c>
+      <c r="C37">
+        <v>15000</v>
+      </c>
+      <c r="D37">
+        <v>2.5</v>
+      </c>
+      <c r="E37">
+        <v>9.5</v>
+      </c>
+      <c r="F37">
+        <v>2.5</v>
+      </c>
+      <c r="G37" t="s">
+        <v>4056</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
+        <v>4045</v>
+      </c>
+      <c r="C38">
+        <v>24000</v>
+      </c>
+      <c r="D38">
+        <v>2.5</v>
+      </c>
+      <c r="E38">
+        <v>11</v>
+      </c>
+      <c r="F38">
+        <v>2.5</v>
+      </c>
+      <c r="G38" t="s">
+        <v>4056</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4046</v>
+      </c>
+      <c r="C39">
+        <v>27000</v>
+      </c>
+      <c r="D39">
+        <v>2.5</v>
+      </c>
+      <c r="E39">
+        <v>13.6</v>
+      </c>
+      <c r="F39">
+        <v>2.5</v>
+      </c>
+      <c r="G39" t="s">
+        <v>4056</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C40">
+        <v>10000</v>
+      </c>
+      <c r="D40">
+        <v>2.5</v>
+      </c>
+      <c r="E40">
+        <v>7.5</v>
+      </c>
+      <c r="F40">
+        <v>2.5</v>
+      </c>
+      <c r="G40" t="s">
+        <v>4056</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C41">
+        <v>10000</v>
+      </c>
+      <c r="D41">
+        <v>2.5</v>
+      </c>
+      <c r="E41">
+        <v>7.5</v>
+      </c>
+      <c r="F41">
+        <v>2.5</v>
+      </c>
+      <c r="G41" t="s">
+        <v>4056</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>4044</v>
+      </c>
+      <c r="C42">
+        <v>15000</v>
+      </c>
+      <c r="D42">
+        <v>2.5</v>
+      </c>
+      <c r="E42">
+        <v>9.5</v>
+      </c>
+      <c r="F42">
+        <v>2.5</v>
+      </c>
+      <c r="G42" t="s">
+        <v>4057</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
+        <v>4045</v>
+      </c>
+      <c r="C43">
+        <v>24000</v>
+      </c>
+      <c r="D43">
+        <v>2.5</v>
+      </c>
+      <c r="E43">
+        <v>11</v>
+      </c>
+      <c r="F43">
+        <v>2.5</v>
+      </c>
+      <c r="G43" t="s">
+        <v>4057</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A44">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>4046</v>
+      </c>
+      <c r="C44">
+        <v>27000</v>
+      </c>
+      <c r="D44">
+        <v>2.5</v>
+      </c>
+      <c r="E44">
+        <v>13.6</v>
+      </c>
+      <c r="F44">
+        <v>2.5</v>
+      </c>
+      <c r="G44" t="s">
+        <v>4057</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A45">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C45">
+        <v>10000</v>
+      </c>
+      <c r="D45">
+        <v>2.5</v>
+      </c>
+      <c r="E45">
+        <v>7.5</v>
+      </c>
+      <c r="F45">
+        <v>2.5</v>
+      </c>
+      <c r="G45" t="s">
+        <v>4057</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C46">
+        <v>10000</v>
+      </c>
+      <c r="D46">
+        <v>2.5</v>
+      </c>
+      <c r="E46">
+        <v>7.5</v>
+      </c>
+      <c r="F46">
+        <v>2.5</v>
+      </c>
+      <c r="G46" t="s">
+        <v>4057</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47">
+        <v>46</v>
+      </c>
+      <c r="B47" t="s">
+        <v>4044</v>
+      </c>
+      <c r="C47">
+        <v>15000</v>
+      </c>
+      <c r="D47">
+        <v>2.5</v>
+      </c>
+      <c r="E47">
+        <v>9.5</v>
+      </c>
+      <c r="F47">
+        <v>2.5</v>
+      </c>
+      <c r="G47" t="s">
+        <v>4057</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>4045</v>
+      </c>
+      <c r="C48">
+        <v>24000</v>
+      </c>
+      <c r="D48">
+        <v>2.5</v>
+      </c>
+      <c r="E48">
+        <v>11</v>
+      </c>
+      <c r="F48">
+        <v>2.5</v>
+      </c>
+      <c r="G48" t="s">
+        <v>4057</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>4046</v>
+      </c>
+      <c r="C49">
+        <v>27000</v>
+      </c>
+      <c r="D49">
+        <v>2.5</v>
+      </c>
+      <c r="E49">
+        <v>13.6</v>
+      </c>
+      <c r="F49">
+        <v>2.5</v>
+      </c>
+      <c r="G49" t="s">
+        <v>4057</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A50">
+        <v>49</v>
+      </c>
+      <c r="B50" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C50">
+        <v>10000</v>
+      </c>
+      <c r="D50">
+        <v>2.5</v>
+      </c>
+      <c r="E50">
+        <v>7.5</v>
+      </c>
+      <c r="F50">
+        <v>2.5</v>
+      </c>
+      <c r="G50" t="s">
+        <v>4057</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A51">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C51">
+        <v>10000</v>
+      </c>
+      <c r="D51">
+        <v>2.5</v>
+      </c>
+      <c r="E51">
+        <v>7.5</v>
+      </c>
+      <c r="F51">
+        <v>2.5</v>
+      </c>
+      <c r="G51" t="s">
+        <v>4057</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A52">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
+        <v>4044</v>
+      </c>
+      <c r="C52">
+        <v>15000</v>
+      </c>
+      <c r="D52">
+        <v>2.5</v>
+      </c>
+      <c r="E52">
+        <v>9.5</v>
+      </c>
+      <c r="F52">
+        <v>2.5</v>
+      </c>
+      <c r="G52" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="53" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A53">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
+        <v>4045</v>
+      </c>
+      <c r="C53">
+        <v>24000</v>
+      </c>
+      <c r="D53">
+        <v>2.5</v>
+      </c>
+      <c r="E53">
+        <v>11</v>
+      </c>
+      <c r="F53">
+        <v>2.5</v>
+      </c>
+      <c r="G53" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="54" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A54">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
+        <v>4046</v>
+      </c>
+      <c r="C54">
+        <v>27000</v>
+      </c>
+      <c r="D54">
+        <v>2.5</v>
+      </c>
+      <c r="E54">
+        <v>13.6</v>
+      </c>
+      <c r="F54">
+        <v>2.5</v>
+      </c>
+      <c r="G54" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="55" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A55">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C55">
+        <v>10000</v>
+      </c>
+      <c r="D55">
+        <v>2.5</v>
+      </c>
+      <c r="E55">
+        <v>7.5</v>
+      </c>
+      <c r="F55">
+        <v>2.5</v>
+      </c>
+      <c r="G55" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="56" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A56">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C56">
+        <v>10000</v>
+      </c>
+      <c r="D56">
+        <v>2.5</v>
+      </c>
+      <c r="E56">
+        <v>7.5</v>
+      </c>
+      <c r="F56">
+        <v>2.5</v>
+      </c>
+      <c r="G56" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A57">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
+        <v>4044</v>
+      </c>
+      <c r="C57">
+        <v>15000</v>
+      </c>
+      <c r="D57">
+        <v>2.5</v>
+      </c>
+      <c r="E57">
+        <v>9.5</v>
+      </c>
+      <c r="F57">
+        <v>2.5</v>
+      </c>
+      <c r="G57" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="58" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A58">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
+        <v>4045</v>
+      </c>
+      <c r="C58">
+        <v>24000</v>
+      </c>
+      <c r="D58">
+        <v>2.5</v>
+      </c>
+      <c r="E58">
+        <v>11</v>
+      </c>
+      <c r="F58">
+        <v>2.5</v>
+      </c>
+      <c r="G58" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="59" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A59">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
+        <v>4046</v>
+      </c>
+      <c r="C59">
+        <v>27000</v>
+      </c>
+      <c r="D59">
+        <v>2.5</v>
+      </c>
+      <c r="E59">
+        <v>13.6</v>
+      </c>
+      <c r="F59">
+        <v>2.5</v>
+      </c>
+      <c r="G59" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A60">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C60">
+        <v>10000</v>
+      </c>
+      <c r="D60">
+        <v>2.5</v>
+      </c>
+      <c r="E60">
+        <v>7.5</v>
+      </c>
+      <c r="F60">
+        <v>2.5</v>
+      </c>
+      <c r="G60" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="61" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A61">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
+        <v>4047</v>
+      </c>
+      <c r="C61">
+        <v>10000</v>
+      </c>
+      <c r="D61">
+        <v>2.5</v>
+      </c>
+      <c r="E61">
+        <v>7.5</v>
+      </c>
+      <c r="F61">
+        <v>2.5</v>
+      </c>
+      <c r="G61" t="s">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -13098,7 +14426,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -13244,7 +14572,7 @@
   <dimension ref="A1:E2001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A11"/>
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -87331,7 +88659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{51214303-FF34-42C9-BF54-D20E5B740810}">
   <dimension ref="A1:C11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
@@ -87356,7 +88684,7 @@
         <v>12</v>
       </c>
       <c r="C2">
-        <f>6371*SQRT((RADIANS(VLOOKUP(B2,customer!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A2,depot!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B2,customer!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A2,depot!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A2,depot!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B2,customer!$A:$D,2,FALSE)))/2)^2))</f>
+        <f>6371*SQRT((RADIANS(VLOOKUP(B2,customers!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A2,depots!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B2,customers!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A2,depots!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A2,depots!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B2,customers!$A:$D,2,FALSE)))/2)^2))</f>
         <v>203.25776947016308</v>
       </c>
     </row>
@@ -87368,7 +88696,7 @@
         <v>14</v>
       </c>
       <c r="C3">
-        <f>6371*SQRT((RADIANS(VLOOKUP(B3,customer!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A3,depot!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B3,customer!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A3,depot!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A3,depot!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B3,customer!$A:$D,2,FALSE)))/2)^2))</f>
+        <f>6371*SQRT((RADIANS(VLOOKUP(B3,customers!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A3,depots!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B3,customers!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A3,depots!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A3,depots!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B3,customers!$A:$D,2,FALSE)))/2)^2))</f>
         <v>56.139133908349606</v>
       </c>
     </row>
@@ -87380,7 +88708,7 @@
         <v>16</v>
       </c>
       <c r="C4">
-        <f>6371*SQRT((RADIANS(VLOOKUP(B4,customer!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A4,depot!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B4,customer!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A4,depot!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A4,depot!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B4,customer!$A:$D,2,FALSE)))/2)^2))</f>
+        <f>6371*SQRT((RADIANS(VLOOKUP(B4,customers!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A4,depots!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B4,customers!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A4,depots!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A4,depots!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B4,customers!$A:$D,2,FALSE)))/2)^2))</f>
         <v>145.82262231558283</v>
       </c>
     </row>
@@ -87392,7 +88720,7 @@
         <v>17</v>
       </c>
       <c r="C5">
-        <f>6371*SQRT((RADIANS(VLOOKUP(B5,customer!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A5,depot!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B5,customer!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A5,depot!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A5,depot!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B5,customer!$A:$D,2,FALSE)))/2)^2))</f>
+        <f>6371*SQRT((RADIANS(VLOOKUP(B5,customers!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A5,depots!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B5,customers!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A5,depots!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A5,depots!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B5,customers!$A:$D,2,FALSE)))/2)^2))</f>
         <v>208.29355311012588</v>
       </c>
     </row>
@@ -87404,7 +88732,7 @@
         <v>18</v>
       </c>
       <c r="C6">
-        <f>6371*SQRT((RADIANS(VLOOKUP(B6,customer!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A6,depot!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B6,customer!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A6,depot!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A6,depot!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B6,customer!$A:$D,2,FALSE)))/2)^2))</f>
+        <f>6371*SQRT((RADIANS(VLOOKUP(B6,customers!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A6,depots!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B6,customers!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A6,depots!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A6,depots!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B6,customers!$A:$D,2,FALSE)))/2)^2))</f>
         <v>106.62208085170491</v>
       </c>
     </row>
@@ -87416,7 +88744,7 @@
         <v>19</v>
       </c>
       <c r="C7">
-        <f>6371*SQRT((RADIANS(VLOOKUP(B7,customer!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A7,depot!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B7,customer!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A7,depot!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A7,depot!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B7,customer!$A:$D,2,FALSE)))/2)^2))</f>
+        <f>6371*SQRT((RADIANS(VLOOKUP(B7,customers!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A7,depots!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B7,customers!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A7,depots!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A7,depots!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B7,customers!$A:$D,2,FALSE)))/2)^2))</f>
         <v>213.54290028226447</v>
       </c>
     </row>
@@ -87428,7 +88756,7 @@
         <v>20</v>
       </c>
       <c r="C8">
-        <f>6371*SQRT((RADIANS(VLOOKUP(B8,customer!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A8,depot!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B8,customer!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A8,depot!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A8,depot!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B8,customer!$A:$D,2,FALSE)))/2)^2))</f>
+        <f>6371*SQRT((RADIANS(VLOOKUP(B8,customers!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A8,depots!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B8,customers!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A8,depots!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A8,depots!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B8,customers!$A:$D,2,FALSE)))/2)^2))</f>
         <v>71.684789635202819</v>
       </c>
     </row>
@@ -87440,7 +88768,7 @@
         <v>21</v>
       </c>
       <c r="C9">
-        <f>6371*SQRT((RADIANS(VLOOKUP(B9,customer!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A9,depot!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B9,customer!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A9,depot!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A9,depot!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B9,customer!$A:$D,2,FALSE)))/2)^2))</f>
+        <f>6371*SQRT((RADIANS(VLOOKUP(B9,customers!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A9,depots!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B9,customers!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A9,depots!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A9,depots!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B9,customers!$A:$D,2,FALSE)))/2)^2))</f>
         <v>222.43665779296379</v>
       </c>
     </row>
@@ -87452,7 +88780,7 @@
         <v>22</v>
       </c>
       <c r="C10">
-        <f>6371*SQRT((RADIANS(VLOOKUP(B10,customer!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A10,depot!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B10,customer!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A10,depot!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A10,depot!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B10,customer!$A:$D,2,FALSE)))/2)^2))</f>
+        <f>6371*SQRT((RADIANS(VLOOKUP(B10,customers!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A10,depots!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B10,customers!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A10,depots!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A10,depots!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B10,customers!$A:$D,2,FALSE)))/2)^2))</f>
         <v>173.85164402856344</v>
       </c>
     </row>
@@ -87464,7 +88792,7 @@
         <v>22</v>
       </c>
       <c r="C11">
-        <f>6371*SQRT((RADIANS(VLOOKUP(B11,customer!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A11,depot!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B11,customer!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A11,depot!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A11,depot!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B11,customer!$A:$D,2,FALSE)))/2)^2))</f>
+        <f>6371*SQRT((RADIANS(VLOOKUP(B11,customers!$A:$D,3,FALSE))-RADIANS(VLOOKUP(A11,depots!$A:$E,3,FALSE)))^2+((RADIANS(VLOOKUP(B11,customers!$A:$D,2,FALSE))-RADIANS(VLOOKUP(A11,depots!$A:$E,2,FALSE)))^2)*(COS((RADIANS(VLOOKUP(A11,depots!$A:$E,2,FALSE))+RADIANS(VLOOKUP(B11,customers!$A:$D,2,FALSE)))/2)^2))</f>
         <v>173.85164402856344</v>
       </c>
     </row>

</xml_diff>

<commit_message>
main data file modified for adding trucks
</commit_message>
<xml_diff>
--- a/data/initial_data_info.xlsx
+++ b/data/initial_data_info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clara.gregori\projects\VisualStudioCode\routing-model-2025\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3717B6D-A8B6-4BA2-9110-A1F20361DE00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7277D82-02F6-4512-A5AA-26A7B7003F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9F6578B3-E217-4A8C-A4A8-11896FE55B29}"/>
   </bookViews>
@@ -12350,7 +12350,7 @@
     <t>EuropeoPetf2</t>
   </si>
   <si>
-    <t>id_type</t>
+    <t>description</t>
   </si>
   <si>
     <t>F4</t>
@@ -12818,13 +12818,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B4B57A9-B49C-41B3-B600-93F9DD029928}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="11.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.88671875" customWidth="1"/>
     <col min="3" max="3" width="19.33203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -14426,7 +14426,7 @@
   <dimension ref="A1:J18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14572,7 +14572,7 @@
   <dimension ref="A1:E2001"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E29" sqref="E29"/>
+      <selection activeCell="A2" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
data bug, trucks vs its original depot arranged
</commit_message>
<xml_diff>
--- a/data/initial_data_info.xlsx
+++ b/data/initial_data_info.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clara.gregori\projects\VisualStudioCode\routing-model-2025\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\clara.gregori\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7277D82-02F6-4512-A5AA-26A7B7003F65}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{936D5661-D73C-407D-A794-9E7363CB1AE7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{9F6578B3-E217-4A8C-A4A8-11896FE55B29}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{9F6578B3-E217-4A8C-A4A8-11896FE55B29}"/>
   </bookViews>
   <sheets>
     <sheet name="trucks" sheetId="1" r:id="rId1"/>
@@ -12818,7 +12818,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6B4B57A9-B49C-41B3-B600-93F9DD029928}">
   <dimension ref="A1:G61"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -14425,8 +14425,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AECEC613-720E-4529-91A3-BF87FC73DF7F}">
   <dimension ref="A1:J18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14473,7 +14473,7 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="B3" s="3">
         <v>41.61553</v>
@@ -14490,7 +14490,7 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" s="3">
         <v>41.808674000000003</v>
@@ -14507,7 +14507,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>4056</v>
       </c>
       <c r="B5" s="3">
         <v>41.476227999999999</v>
@@ -14524,7 +14524,7 @@
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4057</v>
       </c>
       <c r="B6" s="3">
         <v>41.146476323393202</v>
@@ -14541,7 +14541,7 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>2</v>
       </c>
       <c r="B7" s="3">
         <v>41.593169137144102</v>
@@ -42607,7 +42607,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{88E0F8FB-9CB2-4D4E-96A4-F60156D98580}">
   <dimension ref="A1:J2001"/>
   <sheetViews>
-    <sheetView topLeftCell="A1846" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>

</xml_diff>